<commit_message>
fix：pipe filter factory 截取参数问题
</commit_message>
<xml_diff>
--- a/easyexcel-test/src/test/resources/demo/fill/simple.xlsx
+++ b/easyexcel-test/src/test/resources/demo/fill/simple.xlsx
@@ -30,7 +30,7 @@
     <t>忽略</t>
   </si>
   <si>
-    <t>{name | trim}</t>
+    <t>{bulletPoints |  prior-extract:(,&amp;#58),(【,】) | wrapper:blank,blank | list-echo:✅}</t>
   </si>
   <si>
     <t>{number}</t>
@@ -1010,12 +1010,12 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="14.875" customWidth="1"/>
+    <col min="1" max="1" width="84.5" customWidth="1"/>
     <col min="2" max="2" width="11.5" customWidth="1"/>
     <col min="3" max="3" width="24.5" customWidth="1"/>
     <col min="4" max="4" width="25.875" customWidth="1"/>

</xml_diff>